<commit_message>
Added modifier events for the modifier cards, coded-in all monster and weapon cards. TODO: Modifiers
</commit_message>
<xml_diff>
--- a/cards.xlsx
+++ b/cards.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -108,9 +108,6 @@
     <t>Lost Bandit</t>
   </si>
   <si>
-    <t>Skeletal Archer</t>
-  </si>
-  <si>
     <t>Fallen Adventurer</t>
   </si>
   <si>
@@ -132,9 +129,6 @@
     <t>Sewer Rat</t>
   </si>
   <si>
-    <t>Startled Old Hag</t>
-  </si>
-  <si>
     <t>Mutated Bat</t>
   </si>
   <si>
@@ -187,6 +181,12 @@
   </si>
   <si>
     <t>You are debilitated: You lose 1 Def</t>
+  </si>
+  <si>
+    <t>Volatile Goo</t>
+  </si>
+  <si>
+    <t>Hallucination</t>
   </si>
 </sst>
 </file>
@@ -264,21 +264,21 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -286,78 +286,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Нормален" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -367,11 +299,11 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office тема">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Оffice">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="535353"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -407,7 +339,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Оffice">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -479,7 +411,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Оffice">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -655,16 +587,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -673,37 +605,37 @@
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
+    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -719,15 +651,15 @@
       <c r="E4">
         <v>2</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -743,15 +675,15 @@
       <c r="E5">
         <v>2</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -767,15 +699,15 @@
       <c r="E6">
         <v>2</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -791,15 +723,15 @@
       <c r="E7">
         <v>3</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -815,15 +747,15 @@
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -839,54 +771,54 @@
       <c r="E9">
         <v>2</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -900,7 +832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -914,7 +846,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -928,7 +860,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -942,7 +874,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -956,7 +888,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -970,40 +902,40 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C25" s="2" t="s">
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+    </row>
+    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1020,7 +952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1037,9 +969,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="B28">
         <v>17</v>
@@ -1054,9 +986,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B29">
         <v>16</v>
@@ -1071,9 +1003,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30">
         <v>17</v>
@@ -1088,9 +1020,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31">
         <v>15</v>
@@ -1105,9 +1037,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32">
         <v>14</v>
@@ -1122,9 +1054,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33">
         <v>19</v>
@@ -1139,9 +1071,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34">
         <v>13</v>
@@ -1156,9 +1088,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B35">
         <v>15</v>
@@ -1173,9 +1105,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B36">
         <v>14</v>
@@ -1190,9 +1122,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B37">
         <v>18</v>
@@ -1207,9 +1139,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B38">
         <v>21</v>
@@ -1224,9 +1156,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B39">
         <v>10</v>
@@ -1241,9 +1173,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B40">
         <v>17</v>
@@ -1258,97 +1190,108 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B45" s="3" t="s">
+    <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+    </row>
+    <row r="47" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>46</v>
       </c>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="4"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="B47" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+    </row>
+    <row r="48" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+    </row>
+    <row r="49" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+    </row>
+    <row r="50" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>48</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>50</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>52</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>55</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A23:E24"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="F4:J4"/>
+    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="F6:J6"/>
+    <mergeCell ref="F7:J7"/>
+    <mergeCell ref="F8:J8"/>
+    <mergeCell ref="F9:J9"/>
+    <mergeCell ref="A12:E13"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="F14:I14"/>
     <mergeCell ref="B49:F49"/>
     <mergeCell ref="B50:F50"/>
     <mergeCell ref="B45:F45"/>
@@ -1356,17 +1299,6 @@
     <mergeCell ref="B46:F46"/>
     <mergeCell ref="B47:F47"/>
     <mergeCell ref="B48:F48"/>
-    <mergeCell ref="F8:J8"/>
-    <mergeCell ref="F9:J9"/>
-    <mergeCell ref="A12:E13"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="A23:E24"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="F4:J4"/>
-    <mergeCell ref="F5:J5"/>
-    <mergeCell ref="F6:J6"/>
-    <mergeCell ref="F7:J7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1379,7 +1311,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1391,7 +1323,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>